<commit_message>
FEAT nev version v0.3
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Documents\Altium\SimpleFOCDriver\Project Outputs for SimpleFOCDriver\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Documents\Altium\SimpleFOCDriver\Project Outputs for SimpleFOCDriver\SimpleFOCPowerShieldV0.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24315" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-SimpleFOCDriv" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -44,7 +41,7 @@
     <t>PackageReference</t>
   </si>
   <si>
-    <t>VEJ471M1ETR1010</t>
+    <t>RVT1V471M1010 VEJ471M1ETR1010</t>
   </si>
   <si>
     <t/>
@@ -53,157 +50,196 @@
     <t>CAP_PWR</t>
   </si>
   <si>
+    <t>solder_connection</t>
+  </si>
+  <si>
+    <t>SCENC, SCI2C, SCL</t>
+  </si>
+  <si>
+    <t>solder_connection_four</t>
+  </si>
+  <si>
+    <t>SF4, SFA, SFI</t>
+  </si>
+  <si>
+    <t>solder_connection_tripple</t>
+  </si>
+  <si>
+    <t>ST_CS1, ST_CS3, ST1, ST2, ST3, STB</t>
+  </si>
+  <si>
+    <t>TB002-500-03BE</t>
+  </si>
+  <si>
+    <t>TB_MOT</t>
+  </si>
+  <si>
+    <t>TB002-500-02BE</t>
+  </si>
+  <si>
+    <t>TB_PWR</t>
+  </si>
+  <si>
+    <t>BTN8982</t>
+  </si>
+  <si>
+    <t>BTN1, BTN2, BTN3</t>
+  </si>
+  <si>
+    <t>Cap Semi</t>
+  </si>
+  <si>
+    <t>Capacitor (Semiconductor SIM Model)</t>
+  </si>
+  <si>
+    <t>CBY1, CBY3</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>C_IS1, C_IS2, C_IS3</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>C_O1, C_O2, C_O3</t>
+  </si>
+  <si>
+    <t>220nF</t>
+  </si>
+  <si>
+    <t>C_SR1, C_SR2, C_SR3, CL</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>Header, 5-Pin</t>
+  </si>
+  <si>
+    <t>P_ENC</t>
+  </si>
+  <si>
+    <t>Header 6</t>
+  </si>
+  <si>
+    <t>Header, 6-Pin</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Header 8</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin</t>
+  </si>
+  <si>
+    <t>P1, P4</t>
+  </si>
+  <si>
+    <t>Header 10</t>
+  </si>
+  <si>
+    <t>Header, 10-Pin</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>INA240</t>
+  </si>
+  <si>
+    <t>INA1, INA3</t>
+  </si>
+  <si>
+    <t>l7805</t>
+  </si>
+  <si>
+    <t>L78M08</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Res3</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>J1-0603</t>
+  </si>
+  <si>
+    <t>RPA, RPB, RPC</t>
+  </si>
+  <si>
+    <t>3.3K</t>
+  </si>
+  <si>
+    <t>RSCL, RSDA</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>R_CS1, R_CS3</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>RESC6332</t>
+  </si>
+  <si>
+    <t>R_IS1, R_IS2, R_IS3, RL</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R_SR1, R_SR2, R_SR3</t>
+  </si>
+  <si>
+    <t>0.51k</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>Typical BLUE SiC LED</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>3.5X2.8X1.9</t>
+  </si>
+  <si>
     <t>470uF</t>
   </si>
   <si>
-    <t>INA240</t>
-  </si>
-  <si>
-    <t>INA1, INA3</t>
-  </si>
-  <si>
-    <t>solder_connection</t>
-  </si>
-  <si>
-    <t>SCA, SCB, SCC</t>
-  </si>
-  <si>
-    <t>TB002-500-03BE</t>
-  </si>
-  <si>
-    <t>TB_MOT</t>
-  </si>
-  <si>
-    <t>TB002-500-02BE</t>
-  </si>
-  <si>
-    <t>TB_PWR</t>
-  </si>
-  <si>
-    <t>BTN8982</t>
-  </si>
-  <si>
-    <t>BTN1, BTN2, BTN3</t>
-  </si>
-  <si>
-    <t>Cap Semi</t>
-  </si>
-  <si>
-    <t>Capacitor (Semiconductor SIM Model)</t>
-  </si>
-  <si>
-    <t>CBY1, CBY3</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>C0603</t>
-  </si>
-  <si>
-    <t>C_IS1, C_IS2, C_IS3</t>
-  </si>
-  <si>
-    <t>1nF</t>
-  </si>
-  <si>
-    <t>C_SR1, C_SR2, C_SR3</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>Header 5</t>
-  </si>
-  <si>
-    <t>Header, 5-Pin</t>
-  </si>
-  <si>
-    <t>P_ENC</t>
-  </si>
-  <si>
-    <t>Header 6</t>
-  </si>
-  <si>
-    <t>Header, 6-Pin</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Header 8</t>
-  </si>
-  <si>
-    <t>Header, 8-Pin</t>
-  </si>
-  <si>
-    <t>P1, P4</t>
-  </si>
-  <si>
-    <t>Header 10</t>
-  </si>
-  <si>
-    <t>Header, 10-Pin</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>Res3</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>J1-0603</t>
-  </si>
-  <si>
-    <t>RPA, RPB, RPC</t>
-  </si>
-  <si>
-    <t>3.3K</t>
-  </si>
-  <si>
-    <t>R_CS1, R_CS3</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>RESC6332</t>
-  </si>
-  <si>
-    <t>R_IS1, R_IS2, R_IS3, RL</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>R_SR1, R_SR2, R_SR3</t>
-  </si>
-  <si>
-    <t>0.51k</t>
-  </si>
-  <si>
-    <t>LED3</t>
-  </si>
-  <si>
-    <t>Typical BLUE SiC LED</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>3.5X2.8X1.9</t>
+    <t>35V CAP</t>
+  </si>
+  <si>
+    <t>Capacitor (Semiconductor SIM Model) 50V</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -554,15 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -571,159 +609,159 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,16 +769,16 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
@@ -754,216 +792,316 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="3">
+      <c r="F22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="3">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="3">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>59</v>
+      <c r="E25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>